<commit_message>
one hot encoding model factorization AUC
</commit_message>
<xml_diff>
--- a/csv/1_hot_encoding.xlsx
+++ b/csv/1_hot_encoding.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anastassia Kolde\Documents\Israel secondment\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anastassia Kolde\Documents\GitHub\UnstableEpilepsy\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>data</t>
   </si>
@@ -44,16 +44,43 @@
     <t>1st_index</t>
   </si>
   <si>
-    <t>AUC</t>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Carbamazepine</t>
+  </si>
+  <si>
+    <t>Valporate</t>
+  </si>
+  <si>
+    <t>Lamotrigine</t>
+  </si>
+  <si>
+    <t>Levetiracetam</t>
+  </si>
+  <si>
+    <t>Topiramate</t>
+  </si>
+  <si>
+    <t>Oxcarbazepine</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>60/40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,9 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaallaad" xfId="0" builtinId="0"/>
@@ -366,18 +401,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -387,8 +428,26 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -398,8 +457,26 @@
       <c r="C2" s="1">
         <v>0.54213149999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1">
+        <v>0.54616096199999997</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.55380611499999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.50554958825634999</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.63409090908999999</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.78431372549</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.47058823529411697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -409,8 +486,26 @@
       <c r="C3" s="1">
         <v>0.58300640000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>0.61478763933000002</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.63239795917999997</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.64980842900000002</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.63333333329999997</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.14545454545399999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.43770627062700002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -420,8 +515,26 @@
       <c r="C4" s="1">
         <v>0.52062047</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <v>0.5603525211</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.52634803921567996</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.52148720424899997</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.46241134751700003</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.569444444444</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.50245098030000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -430,6 +543,95 @@
       </c>
       <c r="C5" s="1">
         <v>0.58492622999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.54437732342</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.6432160804</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.73949579831930001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.54166666659999996</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.71794871794000004</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.502721088435374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1533</v>
+      </c>
+      <c r="E8" s="3">
+        <v>718</v>
+      </c>
+      <c r="F8" s="3">
+        <v>383</v>
+      </c>
+      <c r="G8" s="3">
+        <v>172</v>
+      </c>
+      <c r="H8" s="3">
+        <v>137</v>
+      </c>
+      <c r="I8" s="3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1112</v>
+      </c>
+      <c r="E9" s="3">
+        <v>523</v>
+      </c>
+      <c r="F9" s="3">
+        <v>320</v>
+      </c>
+      <c r="G9" s="3">
+        <v>154</v>
+      </c>
+      <c r="H9" s="3">
+        <v>100</v>
+      </c>
+      <c r="I9" s="3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>